<commit_message>
full data for NY sites
</commit_message>
<xml_diff>
--- a/csv/Events.xlsx
+++ b/csv/Events.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="9260" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -43,54 +43,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>New York</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>These Canadian titans of sketch comedy continue to influence funny people more than two decades after their CBC/CBS/HBO show went off the air. Here’s hoping at least some old favorites, like the Chicken Lady, the Head Crusher and as many Helens as may fit on one stage, make an appearance. Your best bet for tickets is stubhub.com.</t>
+  </si>
+  <si>
+    <t>Carol Burnett</t>
+  </si>
+  <si>
+    <t>123 W. 43rd St. (43 St/6 Av), Manhattan, NY 10036</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>212-997-1003</t>
+  </si>
+  <si>
+    <t>www.the-townhall-nyc.org</t>
+  </si>
+  <si>
+    <t>The 81-year-old entertainer turns banter with the audience into a whole show. Come prepared with questions for the comedy veteran, and you might just get an answer. For tickets, visit ticketmaster.com.</t>
+  </si>
+  <si>
+    <t>St. George Theatre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>35 Hyatt St. (Hyatt St/Central Av), Staten Island, NY 10301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">718-442-2900 </t>
+  </si>
+  <si>
+    <t>www.stgeorgetheatre.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New York</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>The Kids in the Hall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/8/8e/ETalk2008-Kids_In_The_Hall.jpg</t>
   </si>
   <si>
     <t>The Town Hall</t>
-  </si>
-  <si>
-    <t>These Canadian titans of sketch comedy continue to influence funny people more than two decades after their CBC/CBS/HBO show went off the air. Here’s hoping at least some old favorites, like the Chicken Lady, the Head Crusher and as many Helens as may fit on one stage, make an appearance. Your best bet for tickets is stubhub.com.</t>
-  </si>
-  <si>
-    <t>Carol Burnett</t>
-  </si>
-  <si>
-    <t>123 W. 43rd St. (43 St/6 Av), Manhattan, NY 10036</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>212-997-1003</t>
-  </si>
-  <si>
-    <t>www.the-townhall-nyc.org</t>
-  </si>
-  <si>
-    <t>The 81-year-old entertainer turns banter with the audience into a whole show. Come prepared with questions for the comedy veteran, and you might just get an answer. For tickets, visit ticketmaster.com.</t>
-  </si>
-  <si>
-    <t>St. George Theatre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>35 Hyatt St. (Hyatt St/Central Av), Staten Island, NY 10301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">718-442-2900 </t>
-  </si>
-  <si>
-    <t>www.stgeorgetheatre.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New York</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/8/83/Carol_Burnett_-_1974.jpg</t>
   </si>
 </sst>
 </file>
@@ -149,10 +157,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,7 +183,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="18">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
@@ -177,11 +191,17 @@
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="16" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -510,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -533,7 +553,7 @@
     <col min="16" max="16" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1">
         <v>1</v>
       </c>
@@ -541,60 +561,78 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E1">
         <v>10036</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
       <c r="J1">
         <v>20150501</v>
       </c>
       <c r="N1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>40.755986</v>
+      </c>
+      <c r="Q1">
+        <v>-73.984712000000002</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>10301</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
       </c>
       <c r="J2">
         <v>20150509</v>
       </c>
       <c r="N2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>40.643332999999998</v>
+      </c>
+      <c r="Q2">
+        <v>-74.078889000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 3 colums for sites, add more rows for events
</commit_message>
<xml_diff>
--- a/csv/Events.xlsx
+++ b/csv/Events.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -43,62 +43,150 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>New York</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Carol Burnett</t>
+  </si>
+  <si>
+    <t>123 W. 43rd St. (43 St/6 Av), Manhattan, NY 10036</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>212-997-1003</t>
+  </si>
+  <si>
+    <t>www.the-townhall-nyc.org</t>
+  </si>
+  <si>
+    <t>St. George Theatre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>35 Hyatt St. (Hyatt St/Central Av), Staten Island, NY 10301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">718-442-2900 </t>
+  </si>
+  <si>
+    <t>www.stgeorgetheatre.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New York</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Kids in the Hall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/8/8e/ETalk2008-Kids_In_The_Hall.jpg</t>
+  </si>
+  <si>
+    <t>The Town Hall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/8/83/Carol_Burnett_-_1974.jpg</t>
+  </si>
+  <si>
     <t>These Canadian titans of sketch comedy continue to influence funny people more than two decades after their CBC/CBS/HBO show went off the air. Here’s hoping at least some old favorites, like the Chicken Lady, the Head Crusher and as many Helens as may fit on one stage, make an appearance. Your best bet for tickets is stubhub.com.</t>
-  </si>
-  <si>
-    <t>Carol Burnett</t>
-  </si>
-  <si>
-    <t>123 W. 43rd St. (43 St/6 Av), Manhattan, NY 10036</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>212-997-1003</t>
-  </si>
-  <si>
-    <t>www.the-townhall-nyc.org</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>These Canadian titans of sketch comedy continue to influence funny people more than two decades after their CBC/CBS/HBO show went off the air.</t>
   </si>
   <si>
     <t>The 81-year-old entertainer turns banter with the audience into a whole show. Come prepared with questions for the comedy veteran, and you might just get an answer. For tickets, visit ticketmaster.com.</t>
-  </si>
-  <si>
-    <t>St. George Theatre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>35 Hyatt St. (Hyatt St/Central Av), Staten Island, NY 10301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">718-442-2900 </t>
-  </si>
-  <si>
-    <t>www.stgeorgetheatre.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New York</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Kids in the Hall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/8/8e/ETalk2008-Kids_In_The_Hall.jpg</t>
-  </si>
-  <si>
-    <t>The Town Hall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/8/83/Carol_Burnett_-_1974.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The 81-year-old entertainer turns banter with the audience into a whole show.</t>
+  </si>
+  <si>
+    <t>Dark Universe</t>
+  </si>
+  <si>
+    <t>American Museum of Natural History</t>
+  </si>
+  <si>
+    <t>212-769-5100</t>
+  </si>
+  <si>
+    <t>Central Park West at 79th Street, Manhattan, NY 10024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.nycgo.com/images/460x285/DarkUniverse_AMNH_V1_460x285.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The American Museum of Natural History presents its newest space show, Dark Universe, which celebrates the discoveries that have led us to a greater level of knowledge about our universe, its history and our planet's place in it. Expect breathtaking renderings of cosmic phenomena and spectacular scenes that will make you feel like you've traveled into space. Astrophysicist Neil deGrasse Tyson narrates. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The American Museum of Natural History presents its newest space show.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mapping Brooklyn</t>
+  </si>
+  <si>
+    <t>BRIC House</t>
+  </si>
+  <si>
+    <t>647 Fulton St., Brooklyn, NY 11217</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>718-683-5600</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bricartsmedia.org</t>
+  </si>
+  <si>
+    <t>Mapping Brooklyn features both historic maps and contemporary works of art that make use of mapping and cartography. Among the highlights of the exhibition, which will be on view at BRIC (February 26-May 3) and the Brooklyn Historical Society (February 26-September 6), are a colorful pictorial road map to the 1939 New York World’s Fair, a commercial edition of a Red Scare-era map depicting enclaves of suspected radical activity and a detailed map of one of Brooklyn’s earliest botanic gardens. These are complemented by contemporary works by artists who researched BHS' map collection for their art including pieces by Justin Blinder, Christine Gedeon, Nick Vaughan &amp; Jake Margolin and Sarah Williams.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mapping Brooklyn features both historic maps and contemporary works of art that make use of mapping and cartography. A</t>
+  </si>
+  <si>
+    <t>http://www.nycgo.com/images/460x285/MappingBrooklyn_V1_460x285.jpg</t>
+  </si>
+  <si>
+    <t>Christopher Wool</t>
+  </si>
+  <si>
+    <t>Luhring Augustine</t>
+  </si>
+  <si>
+    <t>531 W 24th St, Manhattan, NY 10011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>212-206-9100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> luhringaugustine.com</t>
+  </si>
+  <si>
+    <t>Best known for his word paintings—dropping vowels in pieces like "TRBL" and "DRNK"—the post-conceptual artist exhibits a new selection of work at this Chelsea gallery. Although Luhring Augustine has yet to announce details, we'd expect a muted palette and immediately discernable point of view. Wool's paintings can be described in many ways, but shy isn't one of them.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post-conceptual artist exhibits a new selection of work at this Chelsea gallery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.nycgo.com/images/460x285/Luhring-Augustine_V1_460x285.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> amnh.org</t>
   </si>
 </sst>
 </file>
@@ -157,10 +245,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -183,7 +283,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="30">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
@@ -194,6 +294,12 @@
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
@@ -202,6 +308,12 @@
     <cellStyle name="超链接" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="28" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -530,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,14 +658,14 @@
     <col min="8" max="8" width="31.5" customWidth="1"/>
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
-    <col min="15" max="15" width="51.5" customWidth="1"/>
-    <col min="16" max="16" width="60.83203125" customWidth="1"/>
+    <col min="12" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="51.5" customWidth="1"/>
+    <col min="17" max="17" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1">
         <v>1</v>
       </c>
@@ -561,78 +673,204 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
       </c>
       <c r="E1">
         <v>10036</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
       <c r="J1">
         <v>20150501</v>
       </c>
       <c r="N1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1">
         <v>40.755986</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>-73.984712000000002</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>10301</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
       <c r="J2">
         <v>20150509</v>
       </c>
       <c r="N2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2">
         <v>40.643332999999998</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>-74.078889000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>10024</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3">
+        <v>20141102</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>11217</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4">
+        <v>20150226</v>
+      </c>
+      <c r="K4">
+        <v>20150926</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5">
+        <v>10011</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5">
+        <v>20150502</v>
+      </c>
+      <c r="K5">
+        <v>20150620</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>